<commit_message>
Project_2 Logisim section done
</commit_message>
<xml_diff>
--- a/Project_2/Logisim/Bird_extended/bird_extension_changes.xlsx
+++ b/Project_2/Logisim/Bird_extended/bird_extension_changes.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rsan\projects\school\CSE4117-Microprocessors\Project_2\Logisim\Bird_extended\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rsan\projects\school\CSE4117-Microprocessors\Project_2\Logisim\Bird_Extended\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAC6B5BD-F307-47D8-A775-AEF21CE1252B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9142350-47F6-46FB-9D05-0F49498E11B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DE8CB966-0C5E-436C-AC6F-D64CE43CCC0D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="80">
   <si>
     <t>Address</t>
   </si>
@@ -95,9 +95,6 @@
     <t>D</t>
   </si>
   <si>
-    <t>E</t>
-  </si>
-  <si>
     <t>FETCH</t>
   </si>
   <si>
@@ -146,9 +143,6 @@
     <t>NEXT_ADDR</t>
   </si>
   <si>
-    <t>0xE</t>
-  </si>
-  <si>
     <t>0xC</t>
   </si>
   <si>
@@ -164,12 +158,6 @@
     <t>16-bit Extended Address Bus Bird CPU Microcode</t>
   </si>
   <si>
-    <t>F</t>
-  </si>
-  <si>
-    <t>0xF</t>
-  </si>
-  <si>
     <t>12-bit Address Bus Bird CPU Machine Code Format</t>
   </si>
   <si>
@@ -245,21 +233,6 @@
     <t>POP2</t>
   </si>
   <si>
-    <t>JMP1</t>
-  </si>
-  <si>
-    <t>JMP2</t>
-  </si>
-  <si>
-    <t>CALL1</t>
-  </si>
-  <si>
-    <t>CALL2</t>
-  </si>
-  <si>
-    <t>0x810</t>
-  </si>
-  <si>
     <t>0x940</t>
   </si>
   <si>
@@ -284,9 +257,6 @@
     <t>0x400C</t>
   </si>
   <si>
-    <t>0x15420</t>
-  </si>
-  <si>
     <t>0x400D</t>
   </si>
   <si>
@@ -296,13 +266,16 @@
     <t>0x9440</t>
   </si>
   <si>
-    <t>0x100E</t>
-  </si>
-  <si>
-    <t>0x1542F</t>
-  </si>
-  <si>
-    <t>0x800</t>
+    <t>0x20810</t>
+  </si>
+  <si>
+    <t>0x5</t>
+  </si>
+  <si>
+    <t>0x12465</t>
+  </si>
+  <si>
+    <t>0x13420</t>
   </si>
 </sst>
 </file>
@@ -433,7 +406,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -472,6 +445,11 @@
       <alignment horizontal="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -573,23 +551,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>462643</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>503463</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>95249</xdr:rowOff>
+      <xdr:rowOff>27213</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>34</xdr:col>
-      <xdr:colOff>190499</xdr:colOff>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>557892</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>66474</xdr:rowOff>
+      <xdr:rowOff>159038</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 4">
+        <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{71083CF9-4DFF-4F4E-A941-EE1F0E4E65AC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{45A24B4D-6C2A-4E53-B83C-C12201ED8464}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -611,8 +589,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11484429" y="1047749"/>
-          <a:ext cx="9524999" cy="7781725"/>
+          <a:off x="10912927" y="979713"/>
+          <a:ext cx="9239251" cy="7942325"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -923,8 +901,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B17C1B6C-1DD3-447E-A634-9FBDC6E555DB}">
   <dimension ref="C1:AP26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="X28" sqref="X28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="V27" sqref="V27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -938,88 +916,88 @@
   </cols>
   <sheetData>
     <row r="1" spans="3:42" x14ac:dyDescent="0.25">
-      <c r="D1" s="19" t="s">
-        <v>56</v>
-      </c>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
-      <c r="L1" s="20"/>
-      <c r="M1" s="20"/>
-      <c r="N1" s="20"/>
-      <c r="O1" s="20"/>
-      <c r="P1" s="20"/>
-      <c r="Q1" s="20"/>
-      <c r="R1" s="20"/>
-      <c r="S1" s="20"/>
+      <c r="D1" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="23"/>
+      <c r="M1" s="23"/>
+      <c r="N1" s="23"/>
+      <c r="O1" s="23"/>
+      <c r="P1" s="23"/>
+      <c r="Q1" s="23"/>
+      <c r="R1" s="23"/>
+      <c r="S1" s="23"/>
     </row>
     <row r="2" spans="3:42" x14ac:dyDescent="0.25">
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20"/>
-      <c r="L2" s="20"/>
-      <c r="M2" s="20"/>
-      <c r="N2" s="20"/>
-      <c r="O2" s="20"/>
-      <c r="P2" s="20"/>
-      <c r="Q2" s="20"/>
-      <c r="R2" s="20"/>
-      <c r="S2" s="20"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
+      <c r="K2" s="23"/>
+      <c r="L2" s="23"/>
+      <c r="M2" s="23"/>
+      <c r="N2" s="23"/>
+      <c r="O2" s="23"/>
+      <c r="P2" s="23"/>
+      <c r="Q2" s="23"/>
+      <c r="R2" s="23"/>
+      <c r="S2" s="23"/>
     </row>
     <row r="3" spans="3:42" x14ac:dyDescent="0.25">
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="20"/>
-      <c r="I3" s="20"/>
-      <c r="J3" s="20"/>
-      <c r="K3" s="20"/>
-      <c r="L3" s="20"/>
-      <c r="M3" s="20"/>
-      <c r="N3" s="20"/>
-      <c r="O3" s="20"/>
-      <c r="P3" s="20"/>
-      <c r="Q3" s="20"/>
-      <c r="R3" s="20"/>
-      <c r="S3" s="20"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
+      <c r="K3" s="23"/>
+      <c r="L3" s="23"/>
+      <c r="M3" s="23"/>
+      <c r="N3" s="23"/>
+      <c r="O3" s="23"/>
+      <c r="P3" s="23"/>
+      <c r="Q3" s="23"/>
+      <c r="R3" s="23"/>
+      <c r="S3" s="23"/>
     </row>
     <row r="8" spans="3:42" x14ac:dyDescent="0.25">
-      <c r="D8" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="18"/>
-      <c r="J8" s="18"/>
-      <c r="K8" s="18"/>
-      <c r="L8" s="18"/>
-      <c r="M8" s="18"/>
-      <c r="N8" s="18"/>
-      <c r="Y8" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="Z8" s="18"/>
-      <c r="AA8" s="18"/>
-      <c r="AB8" s="18"/>
-      <c r="AC8" s="18"/>
-      <c r="AD8" s="18"/>
-      <c r="AE8" s="18"/>
-      <c r="AF8" s="18"/>
-      <c r="AG8" s="18"/>
-      <c r="AH8" s="18"/>
-      <c r="AI8" s="18"/>
+      <c r="D8" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="21"/>
+      <c r="J8" s="21"/>
+      <c r="K8" s="21"/>
+      <c r="L8" s="21"/>
+      <c r="M8" s="21"/>
+      <c r="N8" s="21"/>
+      <c r="Y8" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z8" s="21"/>
+      <c r="AA8" s="21"/>
+      <c r="AB8" s="21"/>
+      <c r="AC8" s="21"/>
+      <c r="AD8" s="21"/>
+      <c r="AE8" s="21"/>
+      <c r="AF8" s="21"/>
+      <c r="AG8" s="21"/>
+      <c r="AH8" s="21"/>
+      <c r="AI8" s="21"/>
     </row>
     <row r="9" spans="3:42" x14ac:dyDescent="0.25">
       <c r="D9" s="5" t="s">
@@ -1068,7 +1046,7 @@
         <v>14</v>
       </c>
       <c r="S9" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="T9" s="1"/>
       <c r="U9" s="1"/>
@@ -1119,111 +1097,113 @@
         <v>14</v>
       </c>
       <c r="AN9" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="3:42" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D10" s="5"/>
       <c r="E10" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="F10" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="F10" s="12" t="s">
+      <c r="G10" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="G10" s="12" t="s">
+      <c r="H10" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="H10" s="12" t="s">
+      <c r="I10" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="I10" s="12" t="s">
+      <c r="J10" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="J10" s="12" t="s">
+      <c r="K10" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="K10" s="12" t="s">
+      <c r="L10" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="L10" s="12" t="s">
+      <c r="M10" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="M10" s="12" t="s">
+      <c r="N10" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="N10" s="12" t="s">
+      <c r="O10" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="O10" s="12" t="s">
+      <c r="P10" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="P10" s="12" t="s">
+      <c r="Q10" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="Q10" s="12" t="s">
+      <c r="R10" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="R10" s="12" t="s">
-        <v>33</v>
-      </c>
       <c r="S10" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Y10" s="5"/>
       <c r="Z10" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="AA10" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="AA10" s="12" t="s">
+      <c r="AB10" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="AB10" s="12" t="s">
+      <c r="AC10" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="AC10" s="12" t="s">
+      <c r="AD10" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="AD10" s="12" t="s">
+      <c r="AE10" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="AE10" s="12" t="s">
+      <c r="AF10" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="AF10" s="12" t="s">
+      <c r="AG10" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="AG10" s="12" t="s">
+      <c r="AH10" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="AH10" s="12" t="s">
+      <c r="AI10" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="AI10" s="12" t="s">
+      <c r="AJ10" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="AJ10" s="12" t="s">
+      <c r="AK10" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="AK10" s="12" t="s">
+      <c r="AL10" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="AL10" s="12" t="s">
+      <c r="AM10" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="AM10" s="12" t="s">
-        <v>33</v>
-      </c>
       <c r="AN10" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="3:42" x14ac:dyDescent="0.25">
       <c r="C11" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D11" s="4">
         <v>0</v>
       </c>
-      <c r="E11" s="2"/>
+      <c r="E11" s="2">
+        <v>1</v>
+      </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
@@ -1242,21 +1222,23 @@
         <v>1</v>
       </c>
       <c r="S11" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="T11" s="10"/>
       <c r="U11" s="10"/>
       <c r="V11" s="10" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="W11" s="10"/>
       <c r="X11" s="17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Y11" s="4">
         <v>0</v>
       </c>
-      <c r="Z11" s="6"/>
+      <c r="Z11" s="6">
+        <v>1</v>
+      </c>
       <c r="AA11" s="6"/>
       <c r="AB11" s="6"/>
       <c r="AC11" s="6"/>
@@ -1275,15 +1257,15 @@
         <v>1</v>
       </c>
       <c r="AN11" s="7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="AP11" s="10" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="12" spans="3:42" x14ac:dyDescent="0.25">
       <c r="C12" s="13" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D12" s="4">
         <v>1</v>
@@ -1309,16 +1291,16 @@
       <c r="Q12" s="8"/>
       <c r="R12" s="8"/>
       <c r="S12" s="9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="T12" s="10"/>
       <c r="U12" s="10"/>
       <c r="V12" s="10" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="W12" s="10"/>
       <c r="X12" s="13" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="Y12" s="4">
         <v>1</v>
@@ -1344,15 +1326,15 @@
       <c r="AL12" s="8"/>
       <c r="AM12" s="8"/>
       <c r="AN12" s="9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="AP12" s="10" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="3:42" x14ac:dyDescent="0.25">
       <c r="C13" s="13" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D13" s="4">
         <v>2</v>
@@ -1378,16 +1360,16 @@
       <c r="Q13" s="2"/>
       <c r="R13" s="2"/>
       <c r="S13" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="T13" s="10"/>
       <c r="U13" s="10"/>
       <c r="V13" s="10" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="W13" s="10"/>
       <c r="X13" s="13" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="Y13" s="4">
         <v>2</v>
@@ -1413,15 +1395,15 @@
       <c r="AL13" s="6"/>
       <c r="AM13" s="6"/>
       <c r="AN13" s="7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="AP13" s="10" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="3:42" x14ac:dyDescent="0.25">
       <c r="C14" s="13" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D14" s="4">
         <v>3</v>
@@ -1445,16 +1427,16 @@
       </c>
       <c r="R14" s="8"/>
       <c r="S14" s="9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="T14" s="10"/>
       <c r="U14" s="10"/>
       <c r="V14" s="10" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="W14" s="10"/>
       <c r="X14" s="13" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="Y14" s="4">
         <v>3</v>
@@ -1473,20 +1455,18 @@
       <c r="AI14" s="8"/>
       <c r="AJ14" s="8"/>
       <c r="AK14" s="8"/>
-      <c r="AL14" s="8">
-        <v>1</v>
-      </c>
+      <c r="AL14" s="8"/>
       <c r="AM14" s="8"/>
       <c r="AN14" s="9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="AP14" s="10" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15" spans="3:42" x14ac:dyDescent="0.25">
       <c r="C15" s="13" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D15" s="4">
         <v>4</v>
@@ -1506,16 +1486,16 @@
       <c r="Q15" s="2"/>
       <c r="R15" s="2"/>
       <c r="S15" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="T15" s="10"/>
       <c r="U15" s="10"/>
       <c r="V15" s="10" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="W15" s="10"/>
       <c r="X15" s="13" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="Y15" s="4">
         <v>4</v>
@@ -1535,15 +1515,15 @@
       <c r="AL15" s="6"/>
       <c r="AM15" s="6"/>
       <c r="AN15" s="7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="AP15" s="10" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="3:42" x14ac:dyDescent="0.25">
       <c r="C16" s="13" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D16" s="4">
         <v>5</v>
@@ -1565,16 +1545,16 @@
       <c r="Q16" s="8"/>
       <c r="R16" s="8"/>
       <c r="S16" s="9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="T16" s="10"/>
       <c r="U16" s="10"/>
       <c r="V16" s="10" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="W16" s="10"/>
       <c r="X16" s="13" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="Y16" s="4">
         <v>5</v>
@@ -1596,10 +1576,10 @@
       <c r="AL16" s="8"/>
       <c r="AM16" s="8"/>
       <c r="AN16" s="9" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="AP16" s="10" t="s">
-        <v>86</v>
+        <v>68</v>
       </c>
     </row>
     <row r="17" spans="3:42" x14ac:dyDescent="0.25">
@@ -1622,12 +1602,12 @@
       <c r="Q17" s="2"/>
       <c r="R17" s="2"/>
       <c r="S17" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="T17" s="10"/>
       <c r="U17" s="10"/>
       <c r="V17" s="10" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="W17" s="10"/>
       <c r="X17" s="13"/>
@@ -1649,15 +1629,15 @@
       <c r="AL17" s="6"/>
       <c r="AM17" s="6"/>
       <c r="AN17" s="7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="AP17" s="10" t="s">
-        <v>78</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="3:42" x14ac:dyDescent="0.25">
       <c r="C18" s="13" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D18" s="4">
         <v>7</v>
@@ -1681,16 +1661,16 @@
       <c r="Q18" s="8"/>
       <c r="R18" s="8"/>
       <c r="S18" s="9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="T18" s="10"/>
       <c r="U18" s="10"/>
       <c r="V18" s="10" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="W18" s="10"/>
       <c r="X18" s="13" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="Y18" s="4">
         <v>7</v>
@@ -1714,15 +1694,15 @@
       <c r="AL18" s="8"/>
       <c r="AM18" s="8"/>
       <c r="AN18" s="9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="AP18" s="10" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
     </row>
     <row r="19" spans="3:42" x14ac:dyDescent="0.25">
       <c r="C19" s="13" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D19" s="4">
         <v>8</v>
@@ -1748,16 +1728,16 @@
       </c>
       <c r="R19" s="2"/>
       <c r="S19" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="T19" s="10"/>
       <c r="U19" s="10"/>
       <c r="V19" s="10" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="W19" s="10"/>
       <c r="X19" s="13" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="Y19" s="4">
         <v>8</v>
@@ -1783,15 +1763,15 @@
       </c>
       <c r="AM19" s="6"/>
       <c r="AN19" s="7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="AP19" s="10" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
     </row>
     <row r="20" spans="3:42" x14ac:dyDescent="0.25">
       <c r="C20" s="13" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D20" s="4">
         <v>9</v>
@@ -1813,13 +1793,13 @@
       <c r="Q20" s="8"/>
       <c r="R20" s="8"/>
       <c r="S20" s="9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="V20" s="10" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="X20" s="13" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="Y20" s="4">
         <v>9</v>
@@ -1841,15 +1821,15 @@
       <c r="AL20" s="8"/>
       <c r="AM20" s="8"/>
       <c r="AN20" s="9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="AP20" s="10" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
     </row>
     <row r="21" spans="3:42" x14ac:dyDescent="0.25">
       <c r="C21" s="13" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>15</v>
@@ -1859,10 +1839,10 @@
         <v>1</v>
       </c>
       <c r="G21" s="2"/>
-      <c r="H21" s="2">
-        <v>1</v>
-      </c>
-      <c r="I21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2">
+        <v>1</v>
+      </c>
       <c r="J21" s="2">
         <v>1</v>
       </c>
@@ -1879,13 +1859,13 @@
       </c>
       <c r="R21" s="2"/>
       <c r="S21" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="V21" s="10" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="X21" s="13" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="Y21" s="4" t="s">
         <v>15</v>
@@ -1895,13 +1875,11 @@
         <v>1</v>
       </c>
       <c r="AB21" s="6"/>
-      <c r="AC21" s="6">
-        <v>1</v>
-      </c>
-      <c r="AD21" s="6"/>
-      <c r="AE21" s="6">
-        <v>1</v>
-      </c>
+      <c r="AC21" s="6"/>
+      <c r="AD21" s="6">
+        <v>1</v>
+      </c>
+      <c r="AE21" s="6"/>
       <c r="AF21" s="6"/>
       <c r="AG21" s="6">
         <v>1</v>
@@ -1909,21 +1887,23 @@
       <c r="AH21" s="6"/>
       <c r="AI21" s="6"/>
       <c r="AJ21" s="6"/>
-      <c r="AK21" s="6"/>
+      <c r="AK21" s="6">
+        <v>1</v>
+      </c>
       <c r="AL21" s="6">
         <v>1</v>
       </c>
       <c r="AM21" s="6"/>
       <c r="AN21" s="7" t="s">
-        <v>43</v>
+        <v>77</v>
       </c>
       <c r="AP21" s="10" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
     </row>
     <row r="22" spans="3:42" x14ac:dyDescent="0.25">
       <c r="C22" s="13" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>16</v>
@@ -1945,13 +1925,13 @@
       <c r="Q22" s="8"/>
       <c r="R22" s="8"/>
       <c r="S22" s="9" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="V22" s="10" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="X22" s="13" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="Y22" s="4" t="s">
         <v>16</v>
@@ -1973,15 +1953,15 @@
       <c r="AL22" s="8"/>
       <c r="AM22" s="8"/>
       <c r="AN22" s="9" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="AP22" s="10" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
     </row>
     <row r="23" spans="3:42" x14ac:dyDescent="0.25">
       <c r="C23" s="13" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>17</v>
@@ -2007,13 +1987,13 @@
       <c r="Q23" s="2"/>
       <c r="R23" s="2"/>
       <c r="S23" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="V23" s="10" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="X23" s="13" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="Y23" s="4" t="s">
         <v>17</v>
@@ -2039,15 +2019,15 @@
       <c r="AL23" s="6"/>
       <c r="AM23" s="6"/>
       <c r="AN23" s="7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="AP23" s="10" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
     </row>
     <row r="24" spans="3:42" x14ac:dyDescent="0.25">
       <c r="C24" s="13" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D24" s="4" t="s">
         <v>18</v>
@@ -2075,13 +2055,13 @@
       <c r="Q24" s="8"/>
       <c r="R24" s="8"/>
       <c r="S24" s="9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="V24" s="10" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="X24" s="13" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="Y24" s="4" t="s">
         <v>18</v>
@@ -2109,72 +2089,55 @@
       <c r="AL24" s="8"/>
       <c r="AM24" s="8"/>
       <c r="AN24" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="AP24" s="10" t="s">
-        <v>85</v>
+        <v>37</v>
+      </c>
+      <c r="AO24" s="20"/>
+      <c r="AP24" s="18" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="25" spans="3:42" x14ac:dyDescent="0.25">
       <c r="D25" s="1"/>
-      <c r="X25" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="Y25" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="Z25" s="6"/>
-      <c r="AA25" s="6"/>
-      <c r="AB25" s="6"/>
-      <c r="AC25" s="6"/>
-      <c r="AD25" s="6"/>
-      <c r="AE25" s="6"/>
-      <c r="AF25" s="6">
-        <v>1</v>
-      </c>
-      <c r="AG25" s="6"/>
-      <c r="AH25" s="6"/>
-      <c r="AI25" s="6"/>
-      <c r="AJ25" s="6"/>
-      <c r="AK25" s="6"/>
-      <c r="AL25" s="6"/>
-      <c r="AM25" s="6"/>
-      <c r="AN25" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="AP25" s="10" t="s">
-        <v>88</v>
-      </c>
+      <c r="X25" s="18"/>
+      <c r="Y25" s="19"/>
+      <c r="Z25" s="19"/>
+      <c r="AA25" s="19"/>
+      <c r="AB25" s="19"/>
+      <c r="AC25" s="19"/>
+      <c r="AD25" s="19"/>
+      <c r="AE25" s="19"/>
+      <c r="AF25" s="19"/>
+      <c r="AG25" s="19"/>
+      <c r="AH25" s="19"/>
+      <c r="AI25" s="19"/>
+      <c r="AJ25" s="19"/>
+      <c r="AK25" s="19"/>
+      <c r="AL25" s="19"/>
+      <c r="AM25" s="19"/>
+      <c r="AN25" s="18"/>
+      <c r="AO25" s="18"/>
+      <c r="AP25" s="18"/>
     </row>
     <row r="26" spans="3:42" x14ac:dyDescent="0.25">
-      <c r="X26" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="Y26" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="Z26" s="14"/>
-      <c r="AA26" s="14"/>
-      <c r="AB26" s="14"/>
-      <c r="AC26" s="14"/>
-      <c r="AD26" s="14"/>
-      <c r="AE26" s="14"/>
-      <c r="AF26" s="14">
-        <v>1</v>
-      </c>
-      <c r="AG26" s="14"/>
-      <c r="AH26" s="14"/>
-      <c r="AI26" s="14"/>
-      <c r="AJ26" s="14"/>
-      <c r="AK26" s="14"/>
-      <c r="AL26" s="14"/>
-      <c r="AM26" s="14"/>
-      <c r="AN26" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="AP26" s="10" t="s">
-        <v>88</v>
-      </c>
+      <c r="X26" s="18"/>
+      <c r="Y26" s="19"/>
+      <c r="Z26" s="19"/>
+      <c r="AA26" s="19"/>
+      <c r="AB26" s="19"/>
+      <c r="AC26" s="19"/>
+      <c r="AD26" s="19"/>
+      <c r="AE26" s="19"/>
+      <c r="AF26" s="19"/>
+      <c r="AG26" s="19"/>
+      <c r="AH26" s="19"/>
+      <c r="AI26" s="19"/>
+      <c r="AJ26" s="19"/>
+      <c r="AK26" s="19"/>
+      <c r="AL26" s="19"/>
+      <c r="AM26" s="19"/>
+      <c r="AN26" s="18"/>
+      <c r="AO26" s="18"/>
+      <c r="AP26" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2193,7 +2156,7 @@
   <dimension ref="C3:AL23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6:I6"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2203,62 +2166,62 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:38" x14ac:dyDescent="0.25">
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="21"/>
+      <c r="L3" s="21"/>
+      <c r="M3" s="21"/>
+      <c r="N3" s="21"/>
+      <c r="O3" s="21"/>
+      <c r="P3" s="21"/>
+      <c r="Q3" s="21"/>
+      <c r="R3" s="21"/>
+      <c r="W3" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="X3" s="21"/>
+      <c r="Y3" s="21"/>
+      <c r="Z3" s="21"/>
+      <c r="AA3" s="21"/>
+      <c r="AB3" s="21"/>
+      <c r="AC3" s="21"/>
+      <c r="AD3" s="21"/>
+      <c r="AE3" s="21"/>
+      <c r="AF3" s="21"/>
+      <c r="AG3" s="21"/>
+      <c r="AH3" s="21"/>
+      <c r="AI3" s="21"/>
+      <c r="AJ3" s="21"/>
+      <c r="AK3" s="21"/>
+      <c r="AL3" s="21"/>
+    </row>
+    <row r="6" spans="3:38" x14ac:dyDescent="0.25">
+      <c r="C6" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
-      <c r="K3" s="18"/>
-      <c r="L3" s="18"/>
-      <c r="M3" s="18"/>
-      <c r="N3" s="18"/>
-      <c r="O3" s="18"/>
-      <c r="P3" s="18"/>
-      <c r="Q3" s="18"/>
-      <c r="R3" s="18"/>
-      <c r="W3" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="X3" s="18"/>
-      <c r="Y3" s="18"/>
-      <c r="Z3" s="18"/>
-      <c r="AA3" s="18"/>
-      <c r="AB3" s="18"/>
-      <c r="AC3" s="18"/>
-      <c r="AD3" s="18"/>
-      <c r="AE3" s="18"/>
-      <c r="AF3" s="18"/>
-      <c r="AG3" s="18"/>
-      <c r="AH3" s="18"/>
-      <c r="AI3" s="18"/>
-      <c r="AJ3" s="18"/>
-      <c r="AK3" s="18"/>
-      <c r="AL3" s="18"/>
-    </row>
-    <row r="6" spans="3:38" x14ac:dyDescent="0.25">
-      <c r="C6" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
-      <c r="F6" s="22"/>
-      <c r="G6" s="22"/>
-      <c r="H6" s="22"/>
-      <c r="I6" s="23"/>
-      <c r="W6" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="X6" s="22"/>
-      <c r="Y6" s="22"/>
-      <c r="Z6" s="22"/>
-      <c r="AA6" s="22"/>
-      <c r="AB6" s="22"/>
-      <c r="AC6" s="23"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="25"/>
+      <c r="H6" s="25"/>
+      <c r="I6" s="26"/>
+      <c r="W6" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="X6" s="25"/>
+      <c r="Y6" s="25"/>
+      <c r="Z6" s="25"/>
+      <c r="AA6" s="25"/>
+      <c r="AB6" s="25"/>
+      <c r="AC6" s="26"/>
     </row>
     <row r="7" spans="3:38" x14ac:dyDescent="0.25">
       <c r="C7" s="14">
@@ -2359,90 +2322,90 @@
       </c>
     </row>
     <row r="8" spans="3:38" x14ac:dyDescent="0.25">
-      <c r="C8" s="24" t="s">
-        <v>45</v>
-      </c>
-      <c r="D8" s="25"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="H8" s="22"/>
-      <c r="I8" s="22"/>
-      <c r="J8" s="22"/>
-      <c r="K8" s="22"/>
-      <c r="L8" s="22"/>
-      <c r="M8" s="22"/>
-      <c r="N8" s="22"/>
-      <c r="O8" s="22"/>
-      <c r="P8" s="22"/>
-      <c r="Q8" s="22"/>
-      <c r="R8" s="23"/>
-      <c r="W8" s="24" t="s">
-        <v>45</v>
-      </c>
-      <c r="X8" s="25"/>
-      <c r="Y8" s="25"/>
-      <c r="Z8" s="26"/>
-      <c r="AA8" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="AB8" s="22"/>
-      <c r="AC8" s="22"/>
-      <c r="AD8" s="22"/>
-      <c r="AE8" s="22"/>
-      <c r="AF8" s="22"/>
-      <c r="AG8" s="22"/>
-      <c r="AH8" s="22"/>
-      <c r="AI8" s="22"/>
-      <c r="AJ8" s="22"/>
-      <c r="AK8" s="22"/>
-      <c r="AL8" s="23"/>
+      <c r="C8" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" s="28"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="H8" s="25"/>
+      <c r="I8" s="25"/>
+      <c r="J8" s="25"/>
+      <c r="K8" s="25"/>
+      <c r="L8" s="25"/>
+      <c r="M8" s="25"/>
+      <c r="N8" s="25"/>
+      <c r="O8" s="25"/>
+      <c r="P8" s="25"/>
+      <c r="Q8" s="25"/>
+      <c r="R8" s="26"/>
+      <c r="W8" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="X8" s="28"/>
+      <c r="Y8" s="28"/>
+      <c r="Z8" s="29"/>
+      <c r="AA8" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB8" s="25"/>
+      <c r="AC8" s="25"/>
+      <c r="AD8" s="25"/>
+      <c r="AE8" s="25"/>
+      <c r="AF8" s="25"/>
+      <c r="AG8" s="25"/>
+      <c r="AH8" s="25"/>
+      <c r="AI8" s="25"/>
+      <c r="AJ8" s="25"/>
+      <c r="AK8" s="25"/>
+      <c r="AL8" s="26"/>
     </row>
     <row r="9" spans="3:38" x14ac:dyDescent="0.25">
       <c r="C9" s="15"/>
       <c r="D9" s="15"/>
       <c r="E9" s="15"/>
       <c r="F9" s="15"/>
-      <c r="W9" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="X9" s="22"/>
-      <c r="Y9" s="22"/>
-      <c r="Z9" s="22"/>
-      <c r="AA9" s="22"/>
-      <c r="AB9" s="22"/>
-      <c r="AC9" s="22"/>
-      <c r="AD9" s="22"/>
-      <c r="AE9" s="22"/>
-      <c r="AF9" s="22"/>
-      <c r="AG9" s="22"/>
-      <c r="AH9" s="22"/>
-      <c r="AI9" s="22"/>
-      <c r="AJ9" s="22"/>
-      <c r="AK9" s="22"/>
-      <c r="AL9" s="23"/>
+      <c r="W9" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="X9" s="25"/>
+      <c r="Y9" s="25"/>
+      <c r="Z9" s="25"/>
+      <c r="AA9" s="25"/>
+      <c r="AB9" s="25"/>
+      <c r="AC9" s="25"/>
+      <c r="AD9" s="25"/>
+      <c r="AE9" s="25"/>
+      <c r="AF9" s="25"/>
+      <c r="AG9" s="25"/>
+      <c r="AH9" s="25"/>
+      <c r="AI9" s="25"/>
+      <c r="AJ9" s="25"/>
+      <c r="AK9" s="25"/>
+      <c r="AL9" s="26"/>
     </row>
     <row r="13" spans="3:38" x14ac:dyDescent="0.25">
-      <c r="C13" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="D13" s="22"/>
-      <c r="E13" s="22"/>
-      <c r="F13" s="22"/>
-      <c r="G13" s="22"/>
-      <c r="H13" s="22"/>
-      <c r="I13" s="23"/>
-      <c r="W13" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="X13" s="22"/>
-      <c r="Y13" s="22"/>
-      <c r="Z13" s="22"/>
-      <c r="AA13" s="22"/>
-      <c r="AB13" s="22"/>
-      <c r="AC13" s="23"/>
+      <c r="C13" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" s="25"/>
+      <c r="E13" s="25"/>
+      <c r="F13" s="25"/>
+      <c r="G13" s="25"/>
+      <c r="H13" s="25"/>
+      <c r="I13" s="26"/>
+      <c r="W13" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="X13" s="25"/>
+      <c r="Y13" s="25"/>
+      <c r="Z13" s="25"/>
+      <c r="AA13" s="25"/>
+      <c r="AB13" s="25"/>
+      <c r="AC13" s="26"/>
     </row>
     <row r="14" spans="3:38" x14ac:dyDescent="0.25">
       <c r="C14" s="14">
@@ -2543,90 +2506,90 @@
       </c>
     </row>
     <row r="15" spans="3:38" x14ac:dyDescent="0.25">
-      <c r="C15" s="24" t="s">
-        <v>52</v>
-      </c>
-      <c r="D15" s="25"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="26"/>
-      <c r="G15" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="H15" s="22"/>
-      <c r="I15" s="22"/>
-      <c r="J15" s="22"/>
-      <c r="K15" s="22"/>
-      <c r="L15" s="22"/>
-      <c r="M15" s="22"/>
-      <c r="N15" s="22"/>
-      <c r="O15" s="22"/>
-      <c r="P15" s="22"/>
-      <c r="Q15" s="22"/>
-      <c r="R15" s="23"/>
-      <c r="W15" s="24" t="s">
-        <v>52</v>
-      </c>
-      <c r="X15" s="25"/>
-      <c r="Y15" s="25"/>
-      <c r="Z15" s="26"/>
-      <c r="AA15" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="AB15" s="22"/>
-      <c r="AC15" s="22"/>
-      <c r="AD15" s="22"/>
-      <c r="AE15" s="22"/>
-      <c r="AF15" s="22"/>
-      <c r="AG15" s="22"/>
-      <c r="AH15" s="22"/>
-      <c r="AI15" s="22"/>
-      <c r="AJ15" s="22"/>
-      <c r="AK15" s="22"/>
-      <c r="AL15" s="23"/>
+      <c r="C15" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="D15" s="28"/>
+      <c r="E15" s="28"/>
+      <c r="F15" s="29"/>
+      <c r="G15" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="H15" s="25"/>
+      <c r="I15" s="25"/>
+      <c r="J15" s="25"/>
+      <c r="K15" s="25"/>
+      <c r="L15" s="25"/>
+      <c r="M15" s="25"/>
+      <c r="N15" s="25"/>
+      <c r="O15" s="25"/>
+      <c r="P15" s="25"/>
+      <c r="Q15" s="25"/>
+      <c r="R15" s="26"/>
+      <c r="W15" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="X15" s="28"/>
+      <c r="Y15" s="28"/>
+      <c r="Z15" s="29"/>
+      <c r="AA15" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB15" s="25"/>
+      <c r="AC15" s="25"/>
+      <c r="AD15" s="25"/>
+      <c r="AE15" s="25"/>
+      <c r="AF15" s="25"/>
+      <c r="AG15" s="25"/>
+      <c r="AH15" s="25"/>
+      <c r="AI15" s="25"/>
+      <c r="AJ15" s="25"/>
+      <c r="AK15" s="25"/>
+      <c r="AL15" s="26"/>
     </row>
     <row r="16" spans="3:38" x14ac:dyDescent="0.25">
       <c r="C16" s="15"/>
       <c r="D16" s="15"/>
       <c r="E16" s="15"/>
       <c r="F16" s="15"/>
-      <c r="W16" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="X16" s="22"/>
-      <c r="Y16" s="22"/>
-      <c r="Z16" s="22"/>
-      <c r="AA16" s="22"/>
-      <c r="AB16" s="22"/>
-      <c r="AC16" s="22"/>
-      <c r="AD16" s="22"/>
-      <c r="AE16" s="22"/>
-      <c r="AF16" s="22"/>
-      <c r="AG16" s="22"/>
-      <c r="AH16" s="22"/>
-      <c r="AI16" s="22"/>
-      <c r="AJ16" s="22"/>
-      <c r="AK16" s="22"/>
-      <c r="AL16" s="23"/>
+      <c r="W16" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="X16" s="25"/>
+      <c r="Y16" s="25"/>
+      <c r="Z16" s="25"/>
+      <c r="AA16" s="25"/>
+      <c r="AB16" s="25"/>
+      <c r="AC16" s="25"/>
+      <c r="AD16" s="25"/>
+      <c r="AE16" s="25"/>
+      <c r="AF16" s="25"/>
+      <c r="AG16" s="25"/>
+      <c r="AH16" s="25"/>
+      <c r="AI16" s="25"/>
+      <c r="AJ16" s="25"/>
+      <c r="AK16" s="25"/>
+      <c r="AL16" s="26"/>
     </row>
     <row r="20" spans="3:38" x14ac:dyDescent="0.25">
-      <c r="C20" s="21" t="s">
-        <v>50</v>
-      </c>
-      <c r="D20" s="22"/>
-      <c r="E20" s="22"/>
-      <c r="F20" s="22"/>
-      <c r="G20" s="22"/>
-      <c r="H20" s="22"/>
-      <c r="I20" s="23"/>
-      <c r="W20" s="21" t="s">
-        <v>50</v>
-      </c>
-      <c r="X20" s="22"/>
-      <c r="Y20" s="22"/>
-      <c r="Z20" s="22"/>
-      <c r="AA20" s="22"/>
-      <c r="AB20" s="22"/>
-      <c r="AC20" s="23"/>
+      <c r="C20" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="D20" s="25"/>
+      <c r="E20" s="25"/>
+      <c r="F20" s="25"/>
+      <c r="G20" s="25"/>
+      <c r="H20" s="25"/>
+      <c r="I20" s="26"/>
+      <c r="W20" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="X20" s="25"/>
+      <c r="Y20" s="25"/>
+      <c r="Z20" s="25"/>
+      <c r="AA20" s="25"/>
+      <c r="AB20" s="25"/>
+      <c r="AC20" s="26"/>
     </row>
     <row r="21" spans="3:38" x14ac:dyDescent="0.25">
       <c r="C21" s="14">
@@ -2727,70 +2690,70 @@
       </c>
     </row>
     <row r="22" spans="3:38" x14ac:dyDescent="0.25">
-      <c r="C22" s="24" t="s">
-        <v>53</v>
-      </c>
-      <c r="D22" s="25"/>
-      <c r="E22" s="25"/>
-      <c r="F22" s="26"/>
-      <c r="G22" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="H22" s="22"/>
-      <c r="I22" s="22"/>
-      <c r="J22" s="22"/>
-      <c r="K22" s="22"/>
-      <c r="L22" s="22"/>
-      <c r="M22" s="22"/>
-      <c r="N22" s="22"/>
-      <c r="O22" s="22"/>
-      <c r="P22" s="22"/>
-      <c r="Q22" s="22"/>
-      <c r="R22" s="23"/>
-      <c r="W22" s="24" t="s">
-        <v>53</v>
-      </c>
-      <c r="X22" s="25"/>
-      <c r="Y22" s="25"/>
-      <c r="Z22" s="26"/>
-      <c r="AA22" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="AB22" s="22"/>
-      <c r="AC22" s="22"/>
-      <c r="AD22" s="22"/>
-      <c r="AE22" s="22"/>
-      <c r="AF22" s="22"/>
-      <c r="AG22" s="22"/>
-      <c r="AH22" s="22"/>
-      <c r="AI22" s="22"/>
-      <c r="AJ22" s="22"/>
-      <c r="AK22" s="22"/>
-      <c r="AL22" s="23"/>
+      <c r="C22" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="D22" s="28"/>
+      <c r="E22" s="28"/>
+      <c r="F22" s="29"/>
+      <c r="G22" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="H22" s="25"/>
+      <c r="I22" s="25"/>
+      <c r="J22" s="25"/>
+      <c r="K22" s="25"/>
+      <c r="L22" s="25"/>
+      <c r="M22" s="25"/>
+      <c r="N22" s="25"/>
+      <c r="O22" s="25"/>
+      <c r="P22" s="25"/>
+      <c r="Q22" s="25"/>
+      <c r="R22" s="26"/>
+      <c r="W22" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="X22" s="28"/>
+      <c r="Y22" s="28"/>
+      <c r="Z22" s="29"/>
+      <c r="AA22" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB22" s="25"/>
+      <c r="AC22" s="25"/>
+      <c r="AD22" s="25"/>
+      <c r="AE22" s="25"/>
+      <c r="AF22" s="25"/>
+      <c r="AG22" s="25"/>
+      <c r="AH22" s="25"/>
+      <c r="AI22" s="25"/>
+      <c r="AJ22" s="25"/>
+      <c r="AK22" s="25"/>
+      <c r="AL22" s="26"/>
     </row>
     <row r="23" spans="3:38" x14ac:dyDescent="0.25">
       <c r="C23" s="15"/>
       <c r="D23" s="15"/>
       <c r="E23" s="15"/>
       <c r="F23" s="15"/>
-      <c r="W23" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="X23" s="18"/>
-      <c r="Y23" s="18"/>
-      <c r="Z23" s="18"/>
-      <c r="AA23" s="18"/>
-      <c r="AB23" s="18"/>
-      <c r="AC23" s="18"/>
-      <c r="AD23" s="18"/>
-      <c r="AE23" s="18"/>
-      <c r="AF23" s="18"/>
-      <c r="AG23" s="18"/>
-      <c r="AH23" s="18"/>
-      <c r="AI23" s="18"/>
-      <c r="AJ23" s="18"/>
-      <c r="AK23" s="18"/>
-      <c r="AL23" s="18"/>
+      <c r="W23" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="X23" s="21"/>
+      <c r="Y23" s="21"/>
+      <c r="Z23" s="21"/>
+      <c r="AA23" s="21"/>
+      <c r="AB23" s="21"/>
+      <c r="AC23" s="21"/>
+      <c r="AD23" s="21"/>
+      <c r="AE23" s="21"/>
+      <c r="AF23" s="21"/>
+      <c r="AG23" s="21"/>
+      <c r="AH23" s="21"/>
+      <c r="AI23" s="21"/>
+      <c r="AJ23" s="21"/>
+      <c r="AK23" s="21"/>
+      <c r="AL23" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="23">
@@ -2826,31 +2789,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08F44E01-63C8-4D12-A31B-13035B39C226}">
   <dimension ref="F4:AC4"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G51" sqref="G51"/>
+    <sheetView topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Y50" sqref="Y50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="4" spans="6:29" x14ac:dyDescent="0.25">
-      <c r="F4" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="27"/>
-      <c r="K4" s="27"/>
-      <c r="L4" s="27"/>
-      <c r="W4" s="27" t="s">
-        <v>55</v>
-      </c>
-      <c r="X4" s="27"/>
-      <c r="Y4" s="27"/>
-      <c r="Z4" s="27"/>
-      <c r="AA4" s="27"/>
-      <c r="AB4" s="27"/>
-      <c r="AC4" s="27"/>
+      <c r="F4" s="30" t="s">
+        <v>50</v>
+      </c>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="30"/>
+      <c r="J4" s="30"/>
+      <c r="K4" s="30"/>
+      <c r="L4" s="30"/>
+      <c r="W4" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="X4" s="30"/>
+      <c r="Y4" s="30"/>
+      <c r="Z4" s="30"/>
+      <c r="AA4" s="30"/>
+      <c r="AB4" s="30"/>
+      <c r="AC4" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>